<commit_message>
Update industry analysis and marketing.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -47,6 +47,54 @@
   </si>
   <si>
     <t>sky{at}cs.berkeley.edu</t>
+  </si>
+  <si>
+    <t>Hongsuk Benjamin Choi</t>
+  </si>
+  <si>
+    <t>https://hongsukchoi.github.io/</t>
+  </si>
+  <si>
+    <t>Chung Min Kim</t>
+  </si>
+  <si>
+    <t>https://chungmin99.github.io/</t>
+  </si>
+  <si>
+    <t>Justin Kerr</t>
+  </si>
+  <si>
+    <t>https://kerrj.github.io/</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Toru Lin</t>
+  </si>
+  <si>
+    <t>https://toruowo.github.io/</t>
+  </si>
+  <si>
+    <t>Production quality modern C++ or Python
+Experience in deep imitation learning or reinforcement learning in realistic applications
+Exposure to robotics learning through tactile and/or vision-based sensors.
+Experience writing both production-level Python (including Numpy and Pytorch) and modern C++
+Proven track record of training and deploying real world neural networks
+Familiarity with 3D computer vision and/or graphics pipelines
+Experience with Natural Language Processing
+Experience with distributed deep learning systems
+Prior work in Robotics, State estimation, Visual Odometry, SLAM, Structure from Motion, 3D Reconstruction</t>
+  </si>
+  <si>
+    <t>In this internship, you’ll:
+Design and develop deep learning models, including Vision Language Models (VLMs) and Large Language Models (LLMs), on real-world sensor data (cameras, LiDAR, radars)
+Explore leveraging VLM’s world knowledge and reasoning capabilities to improve various driving tasks
+Collaborate and work in partnership with research teams across Alphabet
+At a minimum we’d like you to have:
+Pursuing a Masters or PhD program in Computer Science, Electrical Engineering, Machine Learning, or related technical fields
+Experience with Deep Learning, VLM/LLMs, and/or Computer Vision
+Experience with Python and deep learning frameworks such as Jax, Tensorflow, Pytorch</t>
   </si>
 </sst>
 </file>
@@ -76,7 +124,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Cambria"/>
       <charset val="0"/>
     </font>
@@ -675,18 +723,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -999,27 +1050,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="16.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1039,9 +1091,68 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" ht="171" customHeight="1" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="13" ht="198" customHeight="1" spans="1:4">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="https://interact.berkeley.edu/people.html"/>
+    <hyperlink ref="C5" r:id="rId2" display="https://hongsukchoi.github.io/"/>
+    <hyperlink ref="C6" r:id="rId3" display="https://chungmin99.github.io/"/>
+    <hyperlink ref="C7" r:id="rId4" display="https://kerrj.github.io/"/>
+    <hyperlink ref="C8" r:id="rId5" display="https://toruowo.github.io/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[Research DATA200] Update note for lect 11 and research reach out.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="22188" windowHeight="9767" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="RA" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -95,6 +95,51 @@
 Pursuing a Masters or PhD program in Computer Science, Electrical Engineering, Machine Learning, or related technical fields
 Experience with Deep Learning, VLM/LLMs, and/or Computer Vision
 Experience with Python and deep learning frameworks such as Jax, Tensorflow, Pytorch</t>
+  </si>
+  <si>
+    <t>Erdem Bıyık</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>https://ebiyik.github.io/</t>
+  </si>
+  <si>
+    <t>Jesse Thomason</t>
+  </si>
+  <si>
+    <t>https://glamor-usc.github.io/people.html</t>
+  </si>
+  <si>
+    <t>Yue Wang</t>
+  </si>
+  <si>
+    <t>https://yuewang.xyz/</t>
+  </si>
+  <si>
+    <t>Yuke Zhu</t>
+  </si>
+  <si>
+    <t>UTA</t>
+  </si>
+  <si>
+    <t>https://rpl.cs.utexas.edu/</t>
+  </si>
+  <si>
+    <t>Jeannette Bohg</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>https://iprl.stanford.edu/</t>
+  </si>
+  <si>
+    <t>Hao Su</t>
+  </si>
+  <si>
+    <t>UCSD</t>
   </si>
 </sst>
 </file>
@@ -107,7 +152,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +165,13 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Cambria"/>
+      <charset val="0"/>
     </font>
     <font>
       <u/>
@@ -593,147 +645,153 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1052,95 +1110,95 @@
   <sheetPr/>
   <dimension ref="A2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="19.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1296296296296" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.1296296296296" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="14.4" spans="1:3">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="14.4" spans="1:3">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="14.4" spans="1:4">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="14.4" spans="1:3">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="171" customHeight="1" spans="1:4">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="13" ht="198" customHeight="1" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1163,14 +1221,85 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="16.5555555555556" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" display="https://ebiyik.github.io/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -1186,7 +1315,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[DATA200] Update assignment 2.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t>https://maureenzou.github.io/</t>
+  </si>
+  <si>
+    <t>Chelsea Finn</t>
+  </si>
+  <si>
+    <t>https://irislab.stanford.edu//contact.html</t>
+  </si>
+  <si>
+    <t>Dorsa Sadigh</t>
+  </si>
+  <si>
+    <t>https://iliad.stanford.edu/people/</t>
   </si>
 </sst>
 </file>
@@ -210,6 +222,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Cambria"/>
       <charset val="0"/>
     </font>
@@ -217,14 +237,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,6 +379,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -481,12 +505,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -524,12 +542,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,13 +690,13 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -708,16 +720,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -726,78 +738,78 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -808,20 +820,32 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1159,7 +1183,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1183,7 +1207,7 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1191,7 +1215,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1199,7 +1223,7 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1210,25 +1234,25 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="171" customHeight="1" spans="1:4">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="13" ht="198" customHeight="1" spans="1:4">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1251,10 +1275,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -1271,13 +1295,13 @@
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1285,7 +1309,7 @@
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1299,7 +1323,7 @@
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1316,7 +1340,7 @@
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1324,6 +1348,9 @@
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1335,7 +1362,7 @@
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1346,7 +1373,7 @@
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1360,7 +1387,7 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1374,7 +1401,7 @@
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1388,11 +1415,40 @@
       </c>
       <c r="F9" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="https://ebiyik.github.io/"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://rpl.cs.utexas.edu/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[DATA200] Complete fall23 midterm.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>https://iliad.stanford.edu/people/</t>
+  </si>
+  <si>
+    <t>David Held</t>
+  </si>
+  <si>
+    <t>CMU</t>
+  </si>
+  <si>
+    <t>https://davheld.github.io/</t>
+  </si>
+  <si>
+    <t>Deepak Pathak</t>
+  </si>
+  <si>
+    <t>https://www.cs.cmu.edu/~dpathak/#ResearchGroup</t>
+  </si>
+  <si>
+    <t>AV Center</t>
+  </si>
+  <si>
+    <t>https://labs.ri.cmu.edu/av-center/we-are-hiring/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1275,10 +1299,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -1443,6 +1467,44 @@
       </c>
       <c r="D11" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Research]Update reach out list.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960" activeTab="1"/>
+    <workbookView windowWidth="27930" windowHeight="12975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -206,6 +206,28 @@
   </si>
   <si>
     <t>https://labs.ri.cmu.edu/av-center/we-are-hiring/</t>
+  </si>
+  <si>
+    <t>Jiajun Wu</t>
+  </si>
+  <si>
+    <t>https://jiajunwu.com/</t>
+  </si>
+  <si>
+    <t>Pengtao Xie</t>
+  </si>
+  <si>
+    <t>https://pengtaoxie.github.io/</t>
+  </si>
+  <si>
+    <t>My past robotics and computer vision experience mostly spans in practical/industry application at RoboMaster and Momenta, where I realized the importance of providing extra context like language, to solve current autonomous vehicle limitations. That's reason why I want to dive into research before going back to the industry.
+Research Experiences
+• Visual Explainer for Deep Learning Image Classification (NNSFC, 2023–2024):
+In this project, I designed a two-stage image segmentation pipeline and an autoencoder with tree constraints, leveraging Shapley Values to extract and rank image concepts. This approach improved the explanation consistency by 35% across 1,000+ images from 20 ImageNet classes. I also developed a Django-based backend for efficient API handling and built a Vue.js frontend for user authentication, image segmentation, and contribution heatmap visualization.
+• Mining Property Relations of NASICON Solid Electrolyte (NNSFC, 2021–2022):
+I built a BERT-based pipeline to extract over 106,000 entities and 260,000 entity-relation triples from 1,808 research papers. By labeling 7,000+ high-quality sentences, I optimized the NER model, resulting in measurable improvements in precision, recall, and F1-score.
+Relevant Courses
+• At UC Berkeley, I have taken advanced courses such as Computer Vision (with Jitendra Malik), Deep Learning for Computer Vision, Introduction to Robotics, Data Science, and Agentic LLMs. These courses have provided me with a strong theoretical and practical foundation in the techniques and methodologies essential for research.</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -221,7 +243,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +271,13 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -714,7 +743,7 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -723,128 +752,128 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -864,16 +893,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1207,7 +1239,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1231,7 +1263,7 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1239,7 +1271,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1247,7 +1279,7 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1258,25 +1290,25 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="171" customHeight="1" spans="1:4">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="13" ht="198" customHeight="1" spans="1:4">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1299,13 +1331,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
@@ -1502,12 +1534,100 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="6:6">
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" ht="317" customHeight="1" spans="1:7">
+      <c r="A20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="8"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="8"/>
       <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="8"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="8"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:G20"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D1" r:id="rId1" display="https://ebiyik.github.io/"/>
     <hyperlink ref="D4" r:id="rId2" display="https://rpl.cs.utexas.edu/"/>

</xml_diff>

<commit_message>
[Research] Update reach out.
</commit_message>
<xml_diff>
--- a/Research/Reach Out.xlsx
+++ b/Research/Reach Out.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="12975" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t>Vivek Myers</t>
   </si>
@@ -100,6 +100,9 @@
     <t>Erdem Bıyık</t>
   </si>
   <si>
+    <t>Sent</t>
+  </si>
+  <si>
     <t>EMail</t>
   </si>
   <si>
@@ -163,18 +166,15 @@
     <t>https://xiaolonw.github.io/group.html</t>
   </si>
   <si>
+    <t>Xueyan Zou</t>
+  </si>
+  <si>
+    <t>https://maureenzou.github.io/</t>
+  </si>
+  <si>
     <t>LISA/CVPR</t>
   </si>
   <si>
-    <t>Xueyan Zou</t>
-  </si>
-  <si>
-    <t>If xiaolong wang no reponse</t>
-  </si>
-  <si>
-    <t>https://maureenzou.github.io/</t>
-  </si>
-  <si>
     <t>Chelsea Finn</t>
   </si>
   <si>
@@ -218,6 +218,66 @@
   </si>
   <si>
     <t>https://pengtaoxie.github.io/</t>
+  </si>
+  <si>
+    <t>Yilun DU</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>Yunzhu Li</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Kuan Fang</t>
+  </si>
+  <si>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t>https://kuanfang.github.io/join-us.html</t>
+  </si>
+  <si>
+    <t>Yuchen Cui</t>
+  </si>
+  <si>
+    <t>UCLA</t>
+  </si>
+  <si>
+    <t>https://yuchencui.cc/index.html</t>
+  </si>
+  <si>
+    <t>Mingyu Ding</t>
+  </si>
+  <si>
+    <t>UNC</t>
+  </si>
+  <si>
+    <t>https://dingmyu.github.io/</t>
+  </si>
+  <si>
+    <t>Manling Li</t>
+  </si>
+  <si>
+    <t>NWU</t>
+  </si>
+  <si>
+    <t>https://limanling.github.io/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Xianyi Cheng</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>https://xianyicheng.github.io/</t>
   </si>
   <si>
     <t>My past robotics and computer vision experience mostly spans in practical/industry application at RoboMaster and Momenta, where I realized the importance of providing extra context like language, to solve current autonomous vehicle limitations. That's reason why I want to dive into research before going back to the industry.
@@ -230,7 +290,9 @@
 • At UC Berkeley, I have taken advanced courses such as Computer Vision (with Jitendra Malik), Deep Learning for Computer Vision, Introduction to Robotics, Data Science, and Agentic LLMs. These courses have provided me with a strong theoretical and practical foundation in the techniques and methodologies essential for research.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Motivation: My background is in robot perception, where I have worked on 3D vision, object detection, tracking, and robotic navigation. However, through my industry experience, I realized that perception alone is not enough, robots must understand intent and interact naturally with humans. I see VLA as the keystone for the next generation of intelligent robotics, enabling better decision-making, generalization, and human-robot collaboration.
+Future plan: My long-term career goal is to work in the industry as a Computer Vision / Robotics Engineer, focusing on scalable AI-driven robotics/autonomous vehicle solutions. I aim to bridge cutting-edge research with real-world applications, particularly in Vision-Language-Action models and learning-based robotic perception. While I currently do not plan to pursue a PhD, I am highly interested in deepening my research experience in multimodal AI and robotics. My goal is to gain strong hands-on expertise in developing intelligent, adaptive robotic systems that can generalize to real-world environments.
+I am in F-1 visa status, and will be on OPT. I will require a signed letter to indicate my working hours for OPT requirements.</t>
   </si>
 </sst>
 </file>
@@ -273,26 +335,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Cambria"/>
-      <charset val="0"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Cambria"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -432,169 +494,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,13 +805,13 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -773,16 +835,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -791,78 +853,78 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,38 +935,35 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1226,17 +1285,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.1333333333333" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="19.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.1333333333333" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.1333333333333" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -1244,71 +1303,71 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" ht="171" customHeight="1" spans="1:4">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="13" ht="198" customHeight="1" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1331,306 +1390,467 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="12.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="20.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.88333333333333" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3"/>
+    <col min="5" max="5" width="12.75" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+      <c r="E11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E17" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" ht="317" customHeight="1" spans="1:7">
-      <c r="A20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="8"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="8"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="8"/>
-      <c r="F23" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="8"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="8"/>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="8"/>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="8"/>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="8"/>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="8"/>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="8"/>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="8"/>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="8"/>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="8"/>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="8"/>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="8"/>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="8"/>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A20:G20"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="https://ebiyik.github.io/"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://rpl.cs.utexas.edu/"/>
+    <hyperlink ref="E1" r:id="rId1" display="https://ebiyik.github.io/"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://rpl.cs.utexas.edu/"/>
+    <hyperlink ref="E13" r:id="rId3" display="https://davheld.github.io/"/>
+    <hyperlink ref="E14" r:id="rId4" display="https://www.cs.cmu.edu/~dpathak/#ResearchGroup"/>
+    <hyperlink ref="E15" r:id="rId5" display="https://labs.ri.cmu.edu/av-center/we-are-hiring/"/>
+    <hyperlink ref="E17" r:id="rId6" display="https://pengtaoxie.github.io/"/>
+    <hyperlink ref="E21" r:id="rId7" display="https://kuanfang.github.io/join-us.html"/>
+    <hyperlink ref="E24" r:id="rId8" display="https://limanling.github.io/"/>
+    <hyperlink ref="E22" r:id="rId9" display="https://yuchencui.cc/index.html"/>
+    <hyperlink ref="E25" r:id="rId10" display="https://xianyicheng.github.io/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1641,14 +1861,45 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="I1" sqref="I1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="26.3833333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="387" customHeight="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>